<commit_message>
comitting Gates Demo Final
</commit_message>
<xml_diff>
--- a/app/tables/scan_childvacc_822_pg1/forms/scan_childvacc_822_pg1/scan_childvacc_822_pg1.xlsx
+++ b/app/tables/scan_childvacc_822_pg1/forms/scan_childvacc_822_pg1/scan_childvacc_822_pg1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18200" windowHeight="8500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15200" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="68">
   <si>
     <t>setting_name</t>
   </si>
@@ -78,24 +78,15 @@
     <t>reasonsforcare_grid_values</t>
   </si>
   <si>
-    <t>Less than 2.5kg at birth</t>
-  </si>
-  <si>
     <t>Baby is a twin</t>
   </si>
   <si>
-    <t>Baby is bottle-fed</t>
-  </si>
-  <si>
     <t>Mother needs more family support</t>
   </si>
   <si>
     <t>Sibling is underweight</t>
   </si>
   <si>
-    <t>Other reasons (TB, leprosy, social issue, etc.)</t>
-  </si>
-  <si>
     <t>clause</t>
   </si>
   <si>
@@ -216,9 +207,6 @@
     <t>reasonsforcare_image0</t>
   </si>
   <si>
-    <t>select_multiple</t>
-  </si>
-  <si>
     <t>reasonsforcare</t>
   </si>
   <si>
@@ -229,6 +217,15 @@
   </si>
   <si>
     <t>hideInContents</t>
+  </si>
+  <si>
+    <t>Other reasons</t>
+  </si>
+  <si>
+    <t>Baby is bottle fed</t>
+  </si>
+  <si>
+    <t>Less than 2kg at birth</t>
   </si>
 </sst>
 </file>
@@ -569,18 +566,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
@@ -592,23 +586,23 @@
         <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -619,28 +613,28 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -651,28 +645,28 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -683,28 +677,28 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -715,28 +709,28 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="B19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F19" t="b">
         <v>1</v>
@@ -747,28 +741,28 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="B23" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F23" t="b">
         <v>1</v>
@@ -779,28 +773,28 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
@@ -811,28 +805,28 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="B31" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F31" t="b">
         <v>1</v>
@@ -843,28 +837,28 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F35" t="b">
         <v>1</v>
@@ -872,31 +866,31 @@
     </row>
     <row r="36" spans="1:6">
       <c r="B36" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="B39" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -907,28 +901,28 @@
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="B43" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
@@ -939,28 +933,28 @@
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="B47" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F47" t="b">
         <v>1</v>
@@ -971,28 +965,28 @@
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D48" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F51" t="b">
         <v>1</v>
@@ -1003,28 +997,28 @@
         <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D52" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="B55" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C55" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
@@ -1032,13 +1026,13 @@
     </row>
     <row r="56" spans="1:6">
       <c r="B56" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E56" t="s">
         <v>14</v>
@@ -1046,20 +1040,20 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="B59" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C59" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F59" t="b">
         <v>1</v>
@@ -1070,28 +1064,28 @@
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D60" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="B63" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F63" t="b">
         <v>1</v>
@@ -1102,28 +1096,28 @@
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D64" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="B67" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F67" t="b">
         <v>1</v>
@@ -1131,13 +1125,13 @@
     </row>
     <row r="68" spans="1:6">
       <c r="B68" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D68" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E68" t="s">
         <v>17</v>
@@ -1145,20 +1139,20 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="B71" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C71" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F71" t="b">
         <v>1</v>
@@ -1169,15 +1163,15 @@
         <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D72" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1194,9 +1188,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="49.1640625" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -1236,10 +1237,10 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1247,10 +1248,10 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1258,10 +1259,10 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1269,10 +1270,10 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1280,10 +1281,10 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1291,10 +1292,10 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>